<commit_message>
Fixed minor coding issues
</commit_message>
<xml_diff>
--- a/venues2.xlsx
+++ b/venues2.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clorange\Dropbox\CLD\Orange House\FoCoMX\2019 App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\FoCoMX\2019 App\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7D8896-6C6F-4715-9C72-5A4629B444E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="161">
   <si>
     <t>field-content</t>
   </si>
@@ -47,9 +54,6 @@
     <t>https://focomx.focoma.org/venues/aggie-theatre</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Logo%20-%20Aggie%20Theatre%20-%20NEW%20-%202016-03-01_0.png?itok=R5iJWSxn</t>
-  </si>
-  <si>
     <t>All Ages</t>
   </si>
   <si>
@@ -59,36 +63,24 @@
     <t>https://focomx.focoma.org/venues/art-lab-fort-collins</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/art%20lab.jpeg?itok=RFRSMdFz</t>
-  </si>
-  <si>
     <t>Avogadro's Number</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/avogadros-number</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/avos.png?itok=qRSb-VGk</t>
-  </si>
-  <si>
     <t>The Colorado Room</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/colorado-room</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/ColoradoRoom_Logo_Blue_All.jpg?itok=aKdqEBto</t>
-  </si>
-  <si>
     <t>Crooked Stave</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/crooked-stave</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Crooked%20Stave.jpg?itok=-8hVY7bS</t>
-  </si>
-  <si>
     <t>All Ages until 9 PM; 21 + After</t>
   </si>
   <si>
@@ -98,18 +90,12 @@
     <t>https://focomx.focoma.org/venues/downtown-artery</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Downtown-Artery-Logo.jpg?itok=RDes2K4e</t>
-  </si>
-  <si>
     <t>Drunken Monkey</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/drunken-monkey</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/15241950_10154637844286420_7375576792205838741_n_0.jpg?itok=H5yx6yBU</t>
-  </si>
-  <si>
     <t>21+</t>
   </si>
   <si>
@@ -119,45 +105,30 @@
     <t>https://focomx.focoma.org/venues/east-coast</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Screen%20Shot%202018-03-07%20at%202.56.28%20PM.png?itok=ndlTDKMg</t>
-  </si>
-  <si>
     <t>Elliot's Martini Bar</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/elliots-martini-bar</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/logo_1.png?itok=ulEJlwZ5</t>
-  </si>
-  <si>
     <t>Equinox Brewing</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/equinox-brewing</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/485150_10151435467768778_1447358655_n_0.jpg?itok=lGusdeRy</t>
-  </si>
-  <si>
     <t>The Exchange</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/exchange</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/The-Exchange-Logo.jpg?itok=lu2uivFR</t>
-  </si>
-  <si>
     <t>Fort Collins Museum of Discovery - Exhibit Hall</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/fort-collins-museum-discovery-exhibit-hall</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/1492544_10151828129870509_383540134_o.jpg?itok=T21T0_pV</t>
-  </si>
-  <si>
     <t>Fort Collins Museum of Discovery - Otter Box Digital Dome Theater</t>
   </si>
   <si>
@@ -170,90 +141,60 @@
     <t>https://focomx.focoma.org/venues/high-point-bar</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/12226974_189111681424222_1350185311380486957_n.jpg?itok=NUtYzZda</t>
-  </si>
-  <si>
     <t>Hodi's Half Note</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/hodis-half-note</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/1392486_255332781281794_1811140495_n_0.jpg?itok=gPABA12V</t>
-  </si>
-  <si>
     <t>Illegal Pete's</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/illegal-petes</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/illegal-petes.jpg?itok=ILyAXtTu</t>
-  </si>
-  <si>
     <t>Magic Rat</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/magic-rat</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/wEm8WNTH_400x400.jpg?itok=2iSkaC1Y</t>
-  </si>
-  <si>
     <t>The Mayor of Old Town</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/mayor-old-town</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/mayor-man-logo-top.png?itok=h-2ZqOV2</t>
-  </si>
-  <si>
     <t>Metro Urban Food &amp; Booze</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/metro-urban-food-booze</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/39748403_2098037540510108_3391112731594588160_n.png?itok=aRCuLyiJ</t>
-  </si>
-  <si>
     <t>Moe's Original Bar B Que</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/moes-original-bar-b-que</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/moes%20logo.201.shadow.jpg?itok=t-TiVUi0</t>
-  </si>
-  <si>
     <t>The Music District - Living Room</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/music-district-living-room</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Music%20District%20.png?itok=r-T6WJRN</t>
-  </si>
-  <si>
     <t>The Music District - Media Library</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/music-district-media-library</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Music%20District%20_0.png?itok=AGJFGooU</t>
-  </si>
-  <si>
     <t>New Belgium Brewing Co. - Outside</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/new-belgium-brewing-co-outside</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/NBB%20Primary%20logo.jpg?itok=yE7szsWm</t>
-  </si>
-  <si>
     <t>New Belgium Brewing Co. - Tasting Room</t>
   </si>
   <si>
@@ -266,135 +207,90 @@
     <t>https://focomx.focoma.org/venues/odell-brewing-co</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/7967324.odell_.jpg?itok=FuiIH9Se</t>
-  </si>
-  <si>
     <t>The Pizza Press</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/pizza-press</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Hkd3aEQWf-the-pizza-press-logo.png?itok=8PAQMk6J</t>
-  </si>
-  <si>
     <t>Pour Brothers Community Tavern</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/pour-brothers-community-tavern</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/Pour%20Brothers.png?itok=qd58Vx38</t>
-  </si>
-  <si>
     <t>Prost Brewing Co. &amp; Biergarten</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/prost-brewing-co-biergarten</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/prost.png?itok=kMSnea_k</t>
-  </si>
-  <si>
     <t>R Bar and Lounge</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/r-bar-and-lounge</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/12115427_514081075426937_4704883791168680730_n.jpg?itok=HmF1iiQA</t>
-  </si>
-  <si>
     <t>The Rec Room</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/rec-room</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/13432186_1035761479805318_5762394617986370682_n.png?itok=8zzm_2Yl</t>
-  </si>
-  <si>
     <t>The Rickshaw Live</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/rickshaw-live</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/The%20Rickshaw%20Live%20-%20Logo%20-01.jpg?itok=oDNpTvIe</t>
-  </si>
-  <si>
     <t>Scrumpy's Hard Cider Bar and Pub</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/scrumpys-hard-cider-bar-and-pub</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/scrumpys_logo.gif?itok=9pF6TtVB</t>
-  </si>
-  <si>
     <t>Sound Off Silent Disco at Old Town Square</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/sound-silent-disco-old-town-square</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/A9E808D3-C7D1-4E73-AF64-2324DA38E08C.jpeg?itok=Ohd2-gK7</t>
-  </si>
-  <si>
     <t>Surfside 7</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/surfside-7</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/nlCwVNUP_400x400.jpg?itok=37AzOs9i</t>
-  </si>
-  <si>
     <t>Tap and Handle</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/tap-and-handle</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/12140787_1153760524657517_616830684565077063_n.jpg?itok=aAMSbnc6</t>
-  </si>
-  <si>
     <t>Tony's Bar &amp; Rooftop</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/tonys-bar-rooftop</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/14859817_1504585836224736_6506692591175321411_o.jpg?itok=gMQcUiL1</t>
-  </si>
-  <si>
     <t>Washington's</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/washingtons</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/23167957_682180375307398_5358657529379380123_n.jpg?itok=0H2BKnL9</t>
-  </si>
-  <si>
     <t>The Whisk(e)y</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/whiskey</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/the-whiskey.jpg?itok=XwqZVxpI</t>
-  </si>
-  <si>
     <t>Wolverine Farm Letterpress &amp; Publick House</t>
   </si>
   <si>
     <t>https://focomx.focoma.org/venues/wolverine-farm-letterpress-publick-house</t>
   </si>
   <si>
-    <t>https://focomx.focoma.org/sites/default/files/styles/venues/public/newwolverineplustype.jpg?itok=Qg47Bgs6</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -510,12 +406,120 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>img/venues/Logo%20-%20Aggie%20Theatre%20-%20NEW%20-%202016-03-01_0.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/art%20lab.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/avos.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/ColoradoRoom_Logo_Blue_All.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/Crooked%20Stave.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/Downtown-Artery-Logo.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/15241950_10154637844286420_7375576792205838741_n_0.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/Screen%20Shot%202018-03-07%20at%202.56.28%20PM.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/logo_1.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/485150_10151435467768778_1447358655_n_0.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/The-Exchange-Logo.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/1492544_10151828129870509_383540134_o.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/12226974_189111681424222_1350185311380486957_n.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/illegal-petes.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/wEm8WNTH_400x400.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/mayor-man-logo-top.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/39748403_2098037540510108_3391112731594588160_n.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/moes%20logo.201.shadow.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/NBB%20Primary%20logo.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/7967324.odell_.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/Hkd3aEQWf-the-pizza-press-logo.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/Pour%20Brothers.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/prost.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/12115427_514081075426937_4704883791168680730_n.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/13432186_1035761479805318_5762394617986370682_n.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/The%20Rickshaw%20Live%20-%20Logo%20-01.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/A9E808D3-C7D1-4E73-AF64-2324DA38E08C.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/nlCwVNUP_400x400.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/12140787_1153760524657517_616830684565077063_n.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/14859817_1504585836224736_6506692591175321411_o.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/23167957_682180375307398_5358657529379380123_n.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/the-whiskey.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/newwolverineplustype.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/scrumpys_logo.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/hodi.jpg</t>
+  </si>
+  <si>
+    <t>img/venues/MusicDist_living.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,11 +555,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,64 +837,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I40"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="93.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="H1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="G2">
         <v>40.585270000000001</v>
@@ -921,24 +923,24 @@
   },</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>151</v>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>114</v>
       </c>
       <c r="G3">
         <v>40.588839999999998</v>
@@ -967,24 +969,24 @@
   },</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="G4">
         <v>40.579689999999999</v>
@@ -1005,24 +1007,24 @@
   },</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="G5">
         <v>40.57855</v>
@@ -1043,24 +1045,24 @@
   },</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>152</v>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
       </c>
       <c r="G6">
         <v>40.589489999999998</v>
@@ -1081,24 +1083,24 @@
   },</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="G7">
         <v>40.588749999999997</v>
@@ -1119,24 +1121,24 @@
   },</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="G8">
         <v>40.58587</v>
@@ -1157,24 +1159,24 @@
   },</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="G9">
         <v>40.588650000000001</v>
@@ -1195,24 +1197,24 @@
   },</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="G10">
         <v>40.588410000000003</v>
@@ -1233,24 +1235,24 @@
   },</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="1">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="G11">
         <v>40.58625</v>
@@ -1271,24 +1273,24 @@
   },</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="1">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>153</v>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>116</v>
       </c>
       <c r="G12">
         <v>40.589759999999998</v>
@@ -1309,24 +1311,24 @@
   },</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="1">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="G13">
         <v>40.593490000000003</v>
@@ -1347,24 +1349,24 @@
   },</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="1">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="G14">
         <v>40.593490000000003</v>
@@ -1385,24 +1387,24 @@
   },</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="1">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="G15">
         <v>40.588039999999999</v>
@@ -1423,24 +1425,24 @@
   },</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="1">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="G16">
         <v>40.588389999999997</v>
@@ -1461,24 +1463,24 @@
   },</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="1">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="G17">
         <v>40.588000000000001</v>
@@ -1499,24 +1501,24 @@
   },</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="1">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>154</v>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>117</v>
       </c>
       <c r="G18">
         <v>40.587670000000003</v>
@@ -1537,24 +1539,24 @@
   },</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="1">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G19">
         <v>40.587670000000003</v>
@@ -1575,24 +1577,24 @@
   },</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="G20">
         <v>40.586419999999997</v>
@@ -1613,24 +1615,24 @@
   },</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="1">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>8</v>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="G21">
         <v>40.588619999999999</v>
@@ -1651,24 +1653,24 @@
   },</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="1">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>155</v>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>118</v>
       </c>
       <c r="G22">
         <v>40.57873</v>
@@ -1689,24 +1691,24 @@
   },</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="1">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>155</v>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>118</v>
       </c>
       <c r="G23">
         <v>40.57873</v>
@@ -1727,24 +1729,24 @@
   },</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="1">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>8</v>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="G24">
         <v>40.593409999999999</v>
@@ -1765,24 +1767,24 @@
   },</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="1">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>8</v>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="G25">
         <v>40.593409999999999</v>
@@ -1803,24 +1805,24 @@
   },</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="1">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
         <v>25</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>8</v>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="G26">
         <v>40.588900000000002</v>
@@ -1841,24 +1843,24 @@
   },</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="1">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>156</v>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
       </c>
       <c r="G27">
         <v>40.589489999999998</v>
@@ -1879,24 +1881,24 @@
   },</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="1">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28">
         <v>27</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>159</v>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>122</v>
       </c>
       <c r="G28">
         <v>40.588290000000001</v>
@@ -1917,24 +1919,24 @@
   },</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="1">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>28</v>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="G29">
         <v>40.588401400000002</v>
@@ -1955,24 +1957,24 @@
   },</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="1">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>28</v>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="G30">
         <v>40.577889999999996</v>
@@ -1993,24 +1995,24 @@
   },</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="1">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31">
         <v>30</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>28</v>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="G31">
         <v>40.587580000000003</v>
@@ -2031,24 +2033,24 @@
   },</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="1">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32">
         <v>31</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>157</v>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>120</v>
       </c>
       <c r="G32">
         <v>40.581470500000002</v>
@@ -2069,24 +2071,24 @@
   },</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="1">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33">
         <v>32</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>28</v>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="G33">
         <v>40.589489999999998</v>
@@ -2107,24 +2109,24 @@
   },</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="1">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34">
         <v>33</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>158</v>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>121</v>
       </c>
       <c r="G34">
         <v>40.587989999999998</v>
@@ -2145,24 +2147,24 @@
   },</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="1">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35">
         <v>34</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>28</v>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="G35">
         <v>40.588645499999998</v>
@@ -2183,24 +2185,24 @@
   },</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="1">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36">
         <v>35</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="G36">
         <v>40.58381</v>
@@ -2221,24 +2223,24 @@
   },</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="1">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37">
         <v>36</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>28</v>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="G37">
         <v>40.584780000000002</v>
@@ -2259,24 +2261,24 @@
   },</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="1">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38">
         <v>37</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>28</v>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="G38">
         <v>40.589440000000003</v>
@@ -2297,24 +2299,24 @@
   },</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="1">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39">
         <v>38</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>28</v>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="G39">
         <v>40.584899999999998</v>
@@ -2335,24 +2337,24 @@
   },</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="1">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40">
         <v>39</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>8</v>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
       </c>
       <c r="F40" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="G40">
         <v>40.590679999999999</v>

</xml_diff>